<commit_message>
added buckling and experimental wing cross section fea values
</commit_message>
<xml_diff>
--- a/Structure 3 lab/fea_values.xlsx
+++ b/Structure 3 lab/fea_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Aero\Structure 3 lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\OneDrive - Imperial College London\Documents\GitHub\Aero\Structure 3 lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008373DB-2AAC-452A-A56F-F4507D24A0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B63E864-AA62-4CD4-AB7B-D08A7A5F88C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" xr2:uid="{89506378-1B57-4552-91FC-848B1C40344A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{89506378-1B57-4552-91FC-848B1C40344A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Average Numerical Value</t>
   </si>
@@ -107,13 +107,58 @@
     <t>5 cell size</t>
   </si>
   <si>
-    <t>10 Eigenvalues for simplified wing structure</t>
-  </si>
-  <si>
     <t>load @rear spar</t>
   </si>
   <si>
     <t>load @front spar</t>
+  </si>
+  <si>
+    <t>cde</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>ijk</t>
+  </si>
+  <si>
+    <t>Load Nm</t>
+  </si>
+  <si>
+    <t>strain cde 10 cell size</t>
+  </si>
+  <si>
+    <t>strain fgh 10 cell size</t>
+  </si>
+  <si>
+    <t>strain ijk 10 cell size</t>
+  </si>
+  <si>
+    <t>strain cde 5 cell size</t>
+  </si>
+  <si>
+    <t>strain fgh 5 cell size</t>
+  </si>
+  <si>
+    <t>strain ijk 5 cell size</t>
+  </si>
+  <si>
+    <t>Simplified Experimental Wing matches experiment conditions</t>
+  </si>
+  <si>
+    <t>Experimental wing cross section 10 cell size</t>
+  </si>
+  <si>
+    <t>Experimental wing cross section 5 cell size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Eigenvalues for simplified wing structure Buckling </t>
+  </si>
+  <si>
+    <t>Much larger than force of 50lbs</t>
+  </si>
+  <si>
+    <t>Same values but different locations. As it might depend on structure geometery and boundary conditions rather than the load.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +184,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,10 +218,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,28 +561,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA45BFF-399D-45F3-B5DC-270F30EF8628}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="113.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -536,8 +608,17 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -554,14 +635,24 @@
         <v>5.1329999999999998E-6</v>
       </c>
       <c r="F3" s="2">
-        <v>5.0259999999999998E-6</v>
+        <v>5.0200000000000002E-6</v>
       </c>
       <c r="G3" s="2">
         <f>ABS(D3-B3)*100/D3</f>
         <v>9.2645145686934521E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <v>-1.0709399999999999E-5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-1.07044E-5</v>
+      </c>
+      <c r="J3" s="2">
+        <f>ABS(ABS(I3-H3)*100/I3)</f>
+        <v>4.670976420910191E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -584,8 +675,18 @@
         <f t="shared" ref="G4:G6" si="0">ABS(D4-B4)*100/D4</f>
         <v>0.79494274569371826</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2">
+        <v>-3.9143900000000003E-6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-3.9114899999999999E-6</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J6" si="1">ABS(ABS(I4-H4)*100/I4)</f>
+        <v>7.4140544907450354E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -608,8 +709,18 @@
         <f t="shared" si="0"/>
         <v>0.11195527642814003</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <v>-1.8979800000000001E-5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-1.92436E-5</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3708453719678182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -632,13 +743,23 @@
         <f t="shared" si="0"/>
         <v>3.8594040417206897E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <v>-1.6914599999999999E-5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-1.6923100000000001E-5</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0227204235640616E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -652,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -669,7 +790,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -686,7 +807,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -695,7 +816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -705,7 +826,7 @@
         <v>1.6683022571148309</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -723,7 +844,7 @@
         <v>0.69333426515593943</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -741,7 +862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -760,18 +881,18 @@
         <v>1.4229636898920688</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F17" s="2">
         <f>ABS(C11-C21)*100/C11</f>
         <v>0.23819715619384979</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -785,7 +906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -800,7 +921,7 @@
         <v>0.29027576197386468</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -815,12 +936,12 @@
         <v>0.61673701671261694</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -831,7 +952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5740.4</v>
       </c>
@@ -843,19 +964,328 @@
         <v>0.5165560594652332</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>297750</v>
+      </c>
+      <c r="C28" s="2">
+        <v>300457</v>
+      </c>
+      <c r="D28" s="2">
+        <v>306374</v>
+      </c>
+      <c r="E28" s="2">
+        <v>309000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>312000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>320000</v>
+      </c>
+      <c r="H28" s="2">
+        <v>322000</v>
+      </c>
+      <c r="I28" s="2">
+        <v>329000</v>
+      </c>
+      <c r="J28" s="2">
+        <v>332000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2">
+        <v>298000</v>
+      </c>
+      <c r="C29" s="2">
+        <v>300000</v>
+      </c>
+      <c r="D29" s="2">
+        <v>306000</v>
+      </c>
+      <c r="E29" s="2">
+        <v>309000</v>
+      </c>
+      <c r="F29" s="2">
+        <v>312000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>320000</v>
+      </c>
+      <c r="H29" s="2">
+        <v>322000</v>
+      </c>
+      <c r="I29" s="2">
+        <v>329000</v>
+      </c>
+      <c r="J29" s="2">
+        <v>332000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>25</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0</v>
+      </c>
+      <c r="I33" s="7">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13.527567346938699</v>
+      </c>
+      <c r="B34" s="4">
+        <v>-5.29512E-6</v>
+      </c>
+      <c r="C34" s="4">
+        <v>-3.0698099999999997E-5</v>
+      </c>
+      <c r="D34" s="4">
+        <v>-3.0698099999999997E-5</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-5.2911500000000002E-6</v>
+      </c>
+      <c r="F34" s="6">
+        <v>-3.06749E-5</v>
+      </c>
+      <c r="G34" s="6">
+        <v>-3.06749E-5</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" ref="H34:H38" si="2">ABS(ABS(E34-B34)*100/E34)</f>
+        <v>7.503094790357287E-2</v>
+      </c>
+      <c r="I34" s="7">
+        <f>ABS(ABS(F34-C34)*100/F34)</f>
+        <v>7.5631868400538094E-2</v>
+      </c>
+      <c r="J34" s="7">
+        <f>ABS(ABS(G34-D34)*100/G34)</f>
+        <v>7.5631868400538094E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27.055134693877498</v>
+      </c>
+      <c r="B35" s="4">
+        <v>-1.0590200000000001E-5</v>
+      </c>
+      <c r="C35" s="4">
+        <v>-6.1396000000000006E-5</v>
+      </c>
+      <c r="D35" s="4">
+        <v>-6.1396000000000006E-5</v>
+      </c>
+      <c r="E35" s="6">
+        <v>-1.05823E-5</v>
+      </c>
+      <c r="F35" s="6">
+        <v>-6.13496E-5</v>
+      </c>
+      <c r="G35" s="6">
+        <v>-6.13496E-5</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" si="2"/>
+        <v>7.4652958241595693E-2</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" ref="I35:I38" si="3">ABS(ABS(F35-C35)*100/F35)</f>
+        <v>7.5632114960825947E-2</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" ref="J35:J38" si="4">ABS(ABS(G35-D35)*100/G35)</f>
+        <v>7.5632114960825947E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>40.582702040816301</v>
+      </c>
+      <c r="B36" s="4">
+        <v>-1.5885299999999998E-5</v>
+      </c>
+      <c r="C36" s="4">
+        <v>-9.2094099999999996E-5</v>
+      </c>
+      <c r="D36" s="4">
+        <v>-9.2094099999999996E-5</v>
+      </c>
+      <c r="E36" s="6">
+        <v>-1.58734E-5</v>
+      </c>
+      <c r="F36" s="6">
+        <v>-9.2024500000000006E-5</v>
+      </c>
+      <c r="G36" s="6">
+        <v>-9.2024500000000006E-5</v>
+      </c>
+      <c r="H36" s="7">
+        <f t="shared" si="2"/>
+        <v>7.4968185769897999E-2</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="3"/>
+        <v>7.5632032773869984E-2</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="4"/>
+        <v>7.5632032773869984E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>54.110269387755103</v>
+      </c>
+      <c r="B37" s="4">
+        <v>-2.1180400000000001E-5</v>
+      </c>
+      <c r="C37" s="3">
+        <v>-1.2279200000000001E-4</v>
+      </c>
+      <c r="D37" s="3">
+        <v>-1.2279200000000001E-4</v>
+      </c>
+      <c r="E37" s="6">
+        <v>-2.1164600000000001E-5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>-1.2269900000000001E-4</v>
+      </c>
+      <c r="G37" s="5">
+        <v>-1.2269900000000001E-4</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="2"/>
+        <v>7.4652958241595693E-2</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="3"/>
+        <v>7.5795238755002589E-2</v>
+      </c>
+      <c r="J37" s="7">
+        <f t="shared" si="4"/>
+        <v>7.5795238755002589E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>67.637836734693806</v>
+      </c>
+      <c r="B38" s="4">
+        <v>-2.6475500000000001E-5</v>
+      </c>
+      <c r="C38" s="3">
+        <v>-1.5349E-4</v>
+      </c>
+      <c r="D38" s="3">
+        <v>-1.5349E-4</v>
+      </c>
+      <c r="E38" s="6">
+        <v>-2.6455700000000002E-5</v>
+      </c>
+      <c r="F38" s="5">
+        <v>-1.5337400000000001E-4</v>
+      </c>
+      <c r="G38" s="5">
+        <v>-1.5337400000000001E-4</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="2"/>
+        <v>7.484209452027113E-2</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="3"/>
+        <v>7.5632114960803853E-2</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="4"/>
+        <v>7.5632114960803853E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>